<commit_message>
Updated the main.py codes
</commit_message>
<xml_diff>
--- a/outputs/1786501092_BOM.xlsx
+++ b/outputs/1786501092_BOM.xlsx
@@ -14713,7 +14713,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14724,35 +14724,40 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>PrimaryPartNo</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>MatchedPartNo</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Component Description</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>SN/LOT</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>QTY Required</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>QTY Actual</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>IDs</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
@@ -14766,26 +14771,31 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>154581-04</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>IPC, RIGHT, BLK 20, CX-3 2.2.1</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>BSXUFAF000E5</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -14799,26 +14809,31 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>154580-04</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>IPC, LEFT, BLK 20, CX-3 2.2.1</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>BSXUFAE000E5</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -14832,26 +14847,31 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>151043-06</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>ASSY, COMMS, DIVERSE</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>BSXG000005SC</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -14865,26 +14885,31 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>150931-01</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>HARNESS AS, BLUE, CAM AFT - MK30-CX-3</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>BSXR2A002527</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -14898,26 +14923,31 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>150932-01</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>HARNESS AS, PINK, AVIO RIGHT - MK30-CX-3</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
       </c>
       <c r="E6" t="n">
         <v>1</v>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>BSXR2A002183</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -14931,26 +14961,31 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>150933-01</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>HARNESS AS, GREEN, CAM FWD - MK30-CX-3</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>BSXR2A002141</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -14964,26 +14999,31 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>150930-02</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>HARNESS AS, BROWN, AVIO LEFT - MK30-CX-3</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
       </c>
       <c r="E8" t="n">
         <v>1</v>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t>BSXR2A003523</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -14997,27 +15037,32 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>151027-01</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>ASSY, AIR DATA SENSOR</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>1</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>2</v>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>BSXUFAD000V3
 BSXUFAD000V5</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -15031,27 +15076,32 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>151027-01</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>ASSY, AIR DATA SENSOR</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>1</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>2</v>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>BSXUFAD000V3
 BSXUFAD000V5</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -15065,27 +15115,32 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>160272-02</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>PROPELLER ASSY, MK30, OFF-CENTER, CW</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>1</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>2</v>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>BSWU01007067
 BSWU01007089</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -15099,26 +15154,31 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>160275-02</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>PROPELLER ASSY, MK30, CENTER, CCW</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
-      </c>
-      <c r="D12" t="n">
-        <v>1</v>
       </c>
       <c r="E12" t="n">
         <v>1</v>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" t="inlineStr">
         <is>
           <t>BSWU01007334</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -15132,27 +15192,32 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>160273-02</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>PROPELLER ASSY, MK30, OFF-CENTER, CCW</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>1</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>2</v>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>BSWU01007150
 BSWU01007408</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -15166,27 +15231,32 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>160272-02</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>PROPELLER ASSY, MK30, OFF-CENTER, CW</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>1</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>2</v>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>BSWU01007067
 BSWU01007089</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -15200,27 +15270,32 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>160273-02</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>PROPELLER ASSY, MK30, OFF-CENTER, CCW</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>1</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>2</v>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>BSWU01007150
 BSWU01007408</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -15234,26 +15309,31 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>160274-02</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
           <t>PROPELLER ASSY, MK30, CENTER, CW</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
-      </c>
-      <c r="D16" t="n">
-        <v>1</v>
       </c>
       <c r="E16" t="n">
         <v>1</v>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="F16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" t="inlineStr">
         <is>
           <t>BSWU01007273</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -15267,26 +15347,31 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>147702-05</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>ASSY, PDM, CX-3 IAW</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
-      </c>
-      <c r="D17" t="n">
-        <v>1</v>
       </c>
       <c r="E17" t="n">
         <v>1</v>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="F17" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" t="inlineStr">
         <is>
           <t>BSXR2A002090</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -15300,26 +15385,31 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>147080-03</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
           <t>RANGEFINDER, MK30</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
-      </c>
-      <c r="D18" t="n">
-        <v>1</v>
       </c>
       <c r="E18" t="n">
         <v>1</v>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="F18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" t="inlineStr">
         <is>
           <t>BSXBG6537048</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -15333,26 +15423,31 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>153933-01</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
           <t>ASSY, SENSOR LRU, PUMA</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
-      </c>
-      <c r="D19" t="n">
-        <v>1</v>
       </c>
       <c r="E19" t="n">
         <v>1</v>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="F19" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" t="inlineStr">
         <is>
           <t>BSXF042000EL</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -15366,26 +15461,31 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
+          <t>154045-01</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
           <t>ASSY, SENSOR LRU, VISTA</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
-      </c>
-      <c r="D20" t="n">
-        <v>1</v>
       </c>
       <c r="E20" t="n">
         <v>1</v>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="F20" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" t="inlineStr">
         <is>
           <t>BSXF031000CX</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -15399,26 +15499,31 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>156394-02</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
           <t>CX-3 LIGHTING, ASSY, RH, BLK20</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
-      </c>
-      <c r="D21" t="n">
-        <v>1</v>
       </c>
       <c r="E21" t="n">
         <v>1</v>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="F21" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" t="inlineStr">
         <is>
           <t>BSXUFAH001RR</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -15432,47 +15537,57 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>156393-02</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
           <t>CX-3 LIGHTING, ASSY, LH, BLK20</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
-      </c>
-      <c r="D22" t="n">
-        <v>1</v>
       </c>
       <c r="E22" t="n">
         <v>1</v>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="F22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" t="inlineStr">
         <is>
           <t>BSXUFAG001JC</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="H22" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr"/>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>150405-01</t>
+        </is>
+      </c>
       <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr">
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
       </c>
-      <c r="D23" t="n">
+      <c r="E23" t="n">
         <v>1</v>
       </c>
-      <c r="E23" t="n">
+      <c r="F23" t="n">
         <v>0</v>
       </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr">
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr">
         <is>
           <t>NOT FOUND</t>
         </is>
@@ -15486,27 +15601,32 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>147712-03</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
           <t>LRU, MOTOR, CX-3, IAW</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
       </c>
-      <c r="D24" t="n">
+      <c r="E24" t="n">
         <v>1</v>
       </c>
-      <c r="E24" t="n">
+      <c r="F24" t="n">
         <v>2</v>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>BSXE00CBM023
 BSXE00CC1006</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -15520,26 +15640,31 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
+          <t>150416-01</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
           <t>STRUT ASSY, UPR, RH</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
-      </c>
-      <c r="D25" t="n">
-        <v>1</v>
       </c>
       <c r="E25" t="n">
         <v>1</v>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="F25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" t="inlineStr">
         <is>
           <t>BSXWFA00094U</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="H25" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -15553,27 +15678,32 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>147712-03</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
           <t>LRU, MOTOR, CX-3, IAW</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
       </c>
-      <c r="D26" t="n">
+      <c r="E26" t="n">
         <v>1</v>
       </c>
-      <c r="E26" t="n">
+      <c r="F26" t="n">
         <v>2</v>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="G26" t="inlineStr">
         <is>
           <t>BSXE00CBM023
 BSXE00CC1006</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="H26" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -15587,48 +15717,58 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>147712-03</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
           <t>LRU, MOTOR, CX-3, IAW</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
       </c>
-      <c r="D27" t="n">
+      <c r="E27" t="n">
         <v>1</v>
       </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
         <v>2</v>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="G27" t="inlineStr">
         <is>
           <t>BSXE00CBM023
 BSXE00CC1006</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="H27" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr"/>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>150422-01</t>
+        </is>
+      </c>
       <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr">
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
       </c>
-      <c r="D28" t="n">
+      <c r="E28" t="n">
         <v>1</v>
       </c>
-      <c r="E28" t="n">
+      <c r="F28" t="n">
         <v>0</v>
       </c>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr">
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr">
         <is>
           <t>NOT FOUND</t>
         </is>
@@ -15642,48 +15782,58 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
+          <t>147712-03</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
           <t>LRU, MOTOR, CX-3, IAW</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
       </c>
-      <c r="D29" t="n">
+      <c r="E29" t="n">
         <v>1</v>
       </c>
-      <c r="E29" t="n">
+      <c r="F29" t="n">
         <v>2</v>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="G29" t="inlineStr">
         <is>
           <t>BSXE00CBM023
 BSXE00CC1006</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="H29" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr"/>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>150434-01</t>
+        </is>
+      </c>
       <c r="B30" t="inlineStr"/>
-      <c r="C30" t="inlineStr">
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
       </c>
-      <c r="D30" t="n">
+      <c r="E30" t="n">
         <v>1</v>
       </c>
-      <c r="E30" t="n">
+      <c r="F30" t="n">
         <v>0</v>
       </c>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr">
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr">
         <is>
           <t>NOT FOUND</t>
         </is>
@@ -15697,27 +15847,32 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
+          <t>147712-03</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
           <t>LRU, MOTOR, CX-3, IAW</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
       </c>
-      <c r="D31" t="n">
+      <c r="E31" t="n">
         <v>1</v>
       </c>
-      <c r="E31" t="n">
+      <c r="F31" t="n">
         <v>2</v>
       </c>
-      <c r="F31" t="inlineStr">
+      <c r="G31" t="inlineStr">
         <is>
           <t>BSXE00CBM023
 BSXE00CC1006</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr">
+      <c r="H31" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -15731,26 +15886,31 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
+          <t>150446-01</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
           <t>STRUT ASSY, LWR, LH</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
-      </c>
-      <c r="D32" t="n">
-        <v>1</v>
       </c>
       <c r="E32" t="n">
         <v>1</v>
       </c>
-      <c r="F32" t="inlineStr">
+      <c r="F32" t="n">
+        <v>1</v>
+      </c>
+      <c r="G32" t="inlineStr">
         <is>
           <t>BSXWFA0009BF</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr">
+      <c r="H32" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -15764,48 +15924,58 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
+          <t>147712-03</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
           <t>LRU, MOTOR, CX-3, IAW</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
       </c>
-      <c r="D33" t="n">
+      <c r="E33" t="n">
         <v>1</v>
       </c>
-      <c r="E33" t="n">
+      <c r="F33" t="n">
         <v>2</v>
       </c>
-      <c r="F33" t="inlineStr">
+      <c r="G33" t="inlineStr">
         <is>
           <t>BSXE00CBM023
 BSXE00CC1006</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
+      <c r="H33" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr"/>
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>150462-01</t>
+        </is>
+      </c>
       <c r="B34" t="inlineStr"/>
-      <c r="C34" t="inlineStr">
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
       </c>
-      <c r="D34" t="n">
+      <c r="E34" t="n">
         <v>1</v>
       </c>
-      <c r="E34" t="n">
+      <c r="F34" t="n">
         <v>0</v>
       </c>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr">
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr">
         <is>
           <t>NOT FOUND</t>
         </is>
@@ -15819,26 +15989,31 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
+          <t>156976-02</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
           <t>ASSY, FRIDGE, BLK20</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="D35" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
-      </c>
-      <c r="D35" t="n">
-        <v>1</v>
       </c>
       <c r="E35" t="n">
         <v>1</v>
       </c>
-      <c r="F35" t="inlineStr">
+      <c r="F35" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" t="inlineStr">
         <is>
           <t>BSXUFAJ000HR</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr">
+      <c r="H35" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -15852,26 +16027,31 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
+          <t>147838-10</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
           <t>CELLULAR COMMS, MK30</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
-      </c>
-      <c r="D36" t="n">
-        <v>1</v>
       </c>
       <c r="E36" t="n">
         <v>1</v>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="F36" t="n">
+        <v>1</v>
+      </c>
+      <c r="G36" t="inlineStr">
         <is>
           <t>BSXTD2000506</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
+      <c r="H36" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -15885,26 +16065,31 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
+          <t>159860-01</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
           <t>INTEGRATED FAIRING ASSY, UPPER</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
-      </c>
-      <c r="D37" t="n">
-        <v>1</v>
       </c>
       <c r="E37" t="n">
         <v>1</v>
       </c>
-      <c r="F37" t="inlineStr">
+      <c r="F37" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" t="inlineStr">
         <is>
           <t>BS0100008V40</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr">
+      <c r="H37" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -15918,26 +16103,31 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
+          <t>152350-02</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
           <t>FAIRING, BOTTOM ASSY</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D38" t="n">
-        <v>1</v>
       </c>
       <c r="E38" t="n">
         <v>1</v>
       </c>
-      <c r="F38" t="inlineStr">
+      <c r="F38" t="n">
+        <v>1</v>
+      </c>
+      <c r="G38" t="inlineStr">
         <is>
           <t>BLXWFA001ABD (x1)</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr">
+      <c r="H38" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -15951,26 +16141,31 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
+          <t>150308-02</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
           <t>FAIRING, BATTERY, RH, ASSY</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D39" t="n">
-        <v>1</v>
       </c>
       <c r="E39" t="n">
         <v>1</v>
       </c>
-      <c r="F39" t="inlineStr">
+      <c r="F39" t="n">
+        <v>1</v>
+      </c>
+      <c r="G39" t="inlineStr">
         <is>
           <t>BLXWFA0017SX (x1)</t>
         </is>
       </c>
-      <c r="G39" t="inlineStr">
+      <c r="H39" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -15984,26 +16179,31 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
+          <t>150298-02</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
           <t>FAIRING, BATTERY, LH, ASSY</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D40" t="n">
-        <v>1</v>
       </c>
       <c r="E40" t="n">
         <v>1</v>
       </c>
-      <c r="F40" t="inlineStr">
+      <c r="F40" t="n">
+        <v>1</v>
+      </c>
+      <c r="G40" t="inlineStr">
         <is>
           <t>BLXWFA000XJ0 (x1)</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr">
+      <c r="H40" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16017,26 +16217,31 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
+          <t>152347-01</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
           <t>FAIRING, SOB ASSY, LH</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D41" t="n">
-        <v>1</v>
       </c>
       <c r="E41" t="n">
         <v>1</v>
       </c>
-      <c r="F41" t="inlineStr">
+      <c r="F41" t="n">
+        <v>1</v>
+      </c>
+      <c r="G41" t="inlineStr">
         <is>
           <t>BLXWFA000G6S (x1)</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr">
+      <c r="H41" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16050,26 +16255,31 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
+          <t>152349-01</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
           <t>FAIRING, SOB ASSY, RH</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="D42" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D42" t="n">
-        <v>1</v>
       </c>
       <c r="E42" t="n">
         <v>1</v>
       </c>
-      <c r="F42" t="inlineStr">
+      <c r="F42" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" t="inlineStr">
         <is>
           <t>BLXWFA000GWM (x1)</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr">
+      <c r="H42" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16083,26 +16293,31 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
+          <t>152348-01</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
           <t>FAIRING, AFT ASSY, LH</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="D43" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D43" t="n">
-        <v>1</v>
       </c>
       <c r="E43" t="n">
         <v>1</v>
       </c>
-      <c r="F43" t="inlineStr">
+      <c r="F43" t="n">
+        <v>1</v>
+      </c>
+      <c r="G43" t="inlineStr">
         <is>
           <t>BLXWFA00114N (x1)</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr">
+      <c r="H43" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16116,26 +16331,31 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
+          <t>152346-01</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
           <t>FAIRING, AFT ASSY, RH</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D44" t="n">
-        <v>1</v>
       </c>
       <c r="E44" t="n">
         <v>1</v>
       </c>
-      <c r="F44" t="inlineStr">
+      <c r="F44" t="n">
+        <v>1</v>
+      </c>
+      <c r="G44" t="inlineStr">
         <is>
           <t>BLXWFA00195F (x1)</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr">
+      <c r="H44" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16149,26 +16369,31 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
+          <t>152352-02</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
           <t>NOSE CONE ASSY</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="D45" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D45" t="n">
-        <v>1</v>
       </c>
       <c r="E45" t="n">
         <v>1</v>
       </c>
-      <c r="F45" t="inlineStr">
+      <c r="F45" t="n">
+        <v>1</v>
+      </c>
+      <c r="G45" t="inlineStr">
         <is>
           <t>BLXWFA000VET (x1)</t>
         </is>
       </c>
-      <c r="G45" t="inlineStr">
+      <c r="H45" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16182,26 +16407,31 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
+          <t>150483-02</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
           <t>WING ASSY, UPR</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="D46" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D46" t="n">
-        <v>1</v>
       </c>
       <c r="E46" t="n">
         <v>1</v>
       </c>
-      <c r="F46" t="inlineStr">
+      <c r="F46" t="n">
+        <v>1</v>
+      </c>
+      <c r="G46" t="inlineStr">
         <is>
           <t>BLXWFA000TV2 (x1)</t>
         </is>
       </c>
-      <c r="G46" t="inlineStr">
+      <c r="H46" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16215,26 +16445,31 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
+          <t>150479-01</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
           <t>WINGLET ASSY, UPR, LH</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="D47" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D47" t="n">
-        <v>1</v>
       </c>
       <c r="E47" t="n">
         <v>1</v>
       </c>
-      <c r="F47" t="inlineStr">
+      <c r="F47" t="n">
+        <v>1</v>
+      </c>
+      <c r="G47" t="inlineStr">
         <is>
           <t>BLXWFA0017PM (x1)</t>
         </is>
       </c>
-      <c r="G47" t="inlineStr">
+      <c r="H47" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16248,26 +16483,31 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
+          <t>150475-01</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
           <t>WINGLET ASSY, UPR, RH</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="D48" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D48" t="n">
-        <v>1</v>
       </c>
       <c r="E48" t="n">
         <v>1</v>
       </c>
-      <c r="F48" t="inlineStr">
+      <c r="F48" t="n">
+        <v>1</v>
+      </c>
+      <c r="G48" t="inlineStr">
         <is>
           <t>BLXWFA000VQ9 (x1)</t>
         </is>
       </c>
-      <c r="G48" t="inlineStr">
+      <c r="H48" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16281,26 +16521,31 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
+          <t>150503-02</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
           <t>WING ASSY, LWR</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D49" t="n">
-        <v>1</v>
       </c>
       <c r="E49" t="n">
         <v>1</v>
       </c>
-      <c r="F49" t="inlineStr">
+      <c r="F49" t="n">
+        <v>1</v>
+      </c>
+      <c r="G49" t="inlineStr">
         <is>
           <t>BLXWFA001940 (x1)</t>
         </is>
       </c>
-      <c r="G49" t="inlineStr">
+      <c r="H49" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16314,26 +16559,31 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
+          <t>150490-01</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
           <t>WINGLET ASSY, LWR, LH</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="D50" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D50" t="n">
-        <v>1</v>
       </c>
       <c r="E50" t="n">
         <v>1</v>
       </c>
-      <c r="F50" t="inlineStr">
+      <c r="F50" t="n">
+        <v>1</v>
+      </c>
+      <c r="G50" t="inlineStr">
         <is>
           <t>BLXWFA00144M (x1)</t>
         </is>
       </c>
-      <c r="G50" t="inlineStr">
+      <c r="H50" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16347,26 +16597,31 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
+          <t>150494-01</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
           <t>WINGLET ASSY, LWR, RH</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="D51" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D51" t="n">
-        <v>1</v>
       </c>
       <c r="E51" t="n">
         <v>1</v>
       </c>
-      <c r="F51" t="inlineStr">
+      <c r="F51" t="n">
+        <v>1</v>
+      </c>
+      <c r="G51" t="inlineStr">
         <is>
           <t>BLXWFA00191V (x1)</t>
         </is>
       </c>
-      <c r="G51" t="inlineStr">
+      <c r="H51" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16380,26 +16635,31 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
+          <t>150500-02</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
           <t>FAIRING ASSY, WING, LOWER, RH, UPPER SIDE</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
+      <c r="D52" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D52" t="n">
-        <v>1</v>
       </c>
       <c r="E52" t="n">
         <v>1</v>
       </c>
-      <c r="F52" t="inlineStr">
+      <c r="F52" t="n">
+        <v>1</v>
+      </c>
+      <c r="G52" t="inlineStr">
         <is>
           <t>BLXWHF02CF7D (x1)</t>
         </is>
       </c>
-      <c r="G52" t="inlineStr">
+      <c r="H52" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16413,26 +16673,31 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
+          <t>150509-02</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
           <t>FAIRING, WING, LOWER, LH, LOWER SIDE</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="D53" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D53" t="n">
-        <v>1</v>
       </c>
       <c r="E53" t="n">
         <v>1</v>
       </c>
-      <c r="F53" t="inlineStr">
+      <c r="F53" t="n">
+        <v>1</v>
+      </c>
+      <c r="G53" t="inlineStr">
         <is>
           <t>BLXWHF02CBFV (x1)</t>
         </is>
       </c>
-      <c r="G53" t="inlineStr">
+      <c r="H53" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16446,26 +16711,31 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
+          <t>150510-02</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
           <t>FAIRING, WING, LOWER, RH, LOWER SIDE</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="D54" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D54" t="n">
-        <v>1</v>
       </c>
       <c r="E54" t="n">
         <v>1</v>
       </c>
-      <c r="F54" t="inlineStr">
+      <c r="F54" t="n">
+        <v>1</v>
+      </c>
+      <c r="G54" t="inlineStr">
         <is>
           <t>BLXWHF029ANG (x1)</t>
         </is>
       </c>
-      <c r="G54" t="inlineStr">
+      <c r="H54" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16479,26 +16749,31 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
+          <t>150498-02</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
           <t>FAIRING ASSY, WING, LOWER, LH, UPPER SIDE</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
+      <c r="D55" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D55" t="n">
-        <v>1</v>
       </c>
       <c r="E55" t="n">
         <v>1</v>
       </c>
-      <c r="F55" t="inlineStr">
+      <c r="F55" t="n">
+        <v>1</v>
+      </c>
+      <c r="G55" t="inlineStr">
         <is>
           <t>BLXWHF02CF7C (x1)</t>
         </is>
       </c>
-      <c r="G55" t="inlineStr">
+      <c r="H55" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16512,26 +16787,31 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
+          <t>151008-01</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
           <t>SPINNER, MK30, OFF-CENTER</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="D56" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D56" t="n">
-        <v>4</v>
       </c>
       <c r="E56" t="n">
         <v>4</v>
       </c>
-      <c r="F56" t="inlineStr">
+      <c r="F56" t="n">
+        <v>4</v>
+      </c>
+      <c r="G56" t="inlineStr">
         <is>
           <t>BL01000001X5 (x4)</t>
         </is>
       </c>
-      <c r="G56" t="inlineStr">
+      <c r="H56" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16545,26 +16825,31 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
+          <t>151009-01</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
           <t>SPINNER, MK30, CENTER</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="D57" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D57" t="n">
-        <v>2</v>
       </c>
       <c r="E57" t="n">
         <v>2</v>
       </c>
-      <c r="F57" t="inlineStr">
+      <c r="F57" t="n">
+        <v>2</v>
+      </c>
+      <c r="G57" t="inlineStr">
         <is>
           <t>BL01000001WQ (x2)</t>
         </is>
       </c>
-      <c r="G57" t="inlineStr">
+      <c r="H57" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16578,26 +16863,31 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
+          <t>148234-01</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
           <t>LATCH, PUSH-PULL, 0.37" BOLT PROJECTION</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
+      <c r="D58" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D58" t="n">
-        <v>2</v>
       </c>
       <c r="E58" t="n">
         <v>2</v>
       </c>
-      <c r="F58" t="inlineStr">
+      <c r="F58" t="n">
+        <v>2</v>
+      </c>
+      <c r="G58" t="inlineStr">
         <is>
           <t>BL0000001517 (x2)</t>
         </is>
       </c>
-      <c r="G58" t="inlineStr">
+      <c r="H58" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16611,26 +16901,31 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
+          <t>156231-01</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
           <t>FAIRING, MOTOR MOUNT, UPR, INBD, LH</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
+      <c r="D59" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D59" t="n">
-        <v>1</v>
       </c>
       <c r="E59" t="n">
         <v>1</v>
       </c>
-      <c r="F59" t="inlineStr">
+      <c r="F59" t="n">
+        <v>1</v>
+      </c>
+      <c r="G59" t="inlineStr">
         <is>
           <t>BLXWFA000W3D (x1)</t>
         </is>
       </c>
-      <c r="G59" t="inlineStr">
+      <c r="H59" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16644,26 +16939,31 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
+          <t>156234-01</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
           <t>FAIRING, MOTOR MOUNT, UPR, INBD, RH</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
+      <c r="D60" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D60" t="n">
-        <v>1</v>
       </c>
       <c r="E60" t="n">
         <v>1</v>
       </c>
-      <c r="F60" t="inlineStr">
+      <c r="F60" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" t="inlineStr">
         <is>
           <t>BLXWFA0014Q5 (x1)</t>
         </is>
       </c>
-      <c r="G60" t="inlineStr">
+      <c r="H60" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16677,26 +16977,31 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
+          <t>156232-01</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
           <t>FAIRING ASSY, MOTOR MOUNT, UPR, OUTBD, LH</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
+      <c r="D61" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D61" t="n">
-        <v>1</v>
       </c>
       <c r="E61" t="n">
         <v>1</v>
       </c>
-      <c r="F61" t="inlineStr">
+      <c r="F61" t="n">
+        <v>1</v>
+      </c>
+      <c r="G61" t="inlineStr">
         <is>
           <t>BLXWFA000W5H (x1)</t>
         </is>
       </c>
-      <c r="G61" t="inlineStr">
+      <c r="H61" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16710,26 +17015,31 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
+          <t>156235-01</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
           <t>FAIRING ASSY, MOTOR MOUNT, UPR, OUTBD, RH</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
+      <c r="D62" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D62" t="n">
-        <v>1</v>
       </c>
       <c r="E62" t="n">
         <v>1</v>
       </c>
-      <c r="F62" t="inlineStr">
+      <c r="F62" t="n">
+        <v>1</v>
+      </c>
+      <c r="G62" t="inlineStr">
         <is>
           <t>BLXWFA0014QL (x1)</t>
         </is>
       </c>
-      <c r="G62" t="inlineStr">
+      <c r="H62" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16743,26 +17053,31 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
+          <t>150515-02</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
           <t>FAIRING ASSY, WING, UPPER, OUTBD, RH</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
+      <c r="D63" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D63" t="n">
-        <v>1</v>
       </c>
       <c r="E63" t="n">
         <v>1</v>
       </c>
-      <c r="F63" t="inlineStr">
+      <c r="F63" t="n">
+        <v>1</v>
+      </c>
+      <c r="G63" t="inlineStr">
         <is>
           <t>BLXWHF029G3V (x1)</t>
         </is>
       </c>
-      <c r="G63" t="inlineStr">
+      <c r="H63" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16776,26 +17091,31 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
+          <t>150524-02</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
           <t>FAIRING, WING, UPPER, INBD, RH</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr">
+      <c r="D64" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D64" t="n">
-        <v>1</v>
       </c>
       <c r="E64" t="n">
         <v>1</v>
       </c>
-      <c r="F64" t="inlineStr">
+      <c r="F64" t="n">
+        <v>1</v>
+      </c>
+      <c r="G64" t="inlineStr">
         <is>
           <t>BLXWHF029APK (x1)</t>
         </is>
       </c>
-      <c r="G64" t="inlineStr">
+      <c r="H64" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16809,26 +17129,31 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
+          <t>150525-02</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
           <t>FAIRING, WING, UPPER, INBD, LH</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr">
+      <c r="D65" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D65" t="n">
-        <v>1</v>
       </c>
       <c r="E65" t="n">
         <v>1</v>
       </c>
-      <c r="F65" t="inlineStr">
+      <c r="F65" t="n">
+        <v>1</v>
+      </c>
+      <c r="G65" t="inlineStr">
         <is>
           <t>BLXWHF02CBA6 (x1)</t>
         </is>
       </c>
-      <c r="G65" t="inlineStr">
+      <c r="H65" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -16842,110 +17167,135 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
+          <t>150517-02</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
           <t>FAIRING ASSY, WING, UPPER, OUTBD, LH</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr">
+      <c r="D66" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D66" t="n">
-        <v>1</v>
       </c>
       <c r="E66" t="n">
         <v>1</v>
       </c>
-      <c r="F66" t="inlineStr">
+      <c r="F66" t="n">
+        <v>1</v>
+      </c>
+      <c r="G66" t="inlineStr">
         <is>
           <t>BLXWHF02CF7A (x1)</t>
         </is>
       </c>
-      <c r="G66" t="inlineStr">
+      <c r="H66" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr"/>
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>156228-01</t>
+        </is>
+      </c>
       <c r="B67" t="inlineStr"/>
-      <c r="C67" t="inlineStr">
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
       </c>
-      <c r="D67" t="n">
+      <c r="E67" t="n">
         <v>1</v>
       </c>
-      <c r="E67" t="n">
+      <c r="F67" t="n">
         <v>0</v>
       </c>
-      <c r="F67" t="inlineStr"/>
-      <c r="G67" t="inlineStr">
+      <c r="G67" t="inlineStr"/>
+      <c r="H67" t="inlineStr">
         <is>
           <t>NOT FOUND</t>
         </is>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr"/>
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>156227-01</t>
+        </is>
+      </c>
       <c r="B68" t="inlineStr"/>
-      <c r="C68" t="inlineStr">
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
       </c>
-      <c r="D68" t="n">
+      <c r="E68" t="n">
         <v>1</v>
       </c>
-      <c r="E68" t="n">
+      <c r="F68" t="n">
         <v>0</v>
       </c>
-      <c r="F68" t="inlineStr"/>
-      <c r="G68" t="inlineStr">
+      <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr">
         <is>
           <t>NOT FOUND</t>
         </is>
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr"/>
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>156224-01</t>
+        </is>
+      </c>
       <c r="B69" t="inlineStr"/>
-      <c r="C69" t="inlineStr">
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
       </c>
-      <c r="D69" t="n">
+      <c r="E69" t="n">
         <v>1</v>
       </c>
-      <c r="E69" t="n">
+      <c r="F69" t="n">
         <v>0</v>
       </c>
-      <c r="F69" t="inlineStr"/>
-      <c r="G69" t="inlineStr">
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr">
         <is>
           <t>NOT FOUND</t>
         </is>
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr"/>
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>156223-01</t>
+        </is>
+      </c>
       <c r="B70" t="inlineStr"/>
-      <c r="C70" t="inlineStr">
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
       </c>
-      <c r="D70" t="n">
+      <c r="E70" t="n">
         <v>1</v>
       </c>
-      <c r="E70" t="n">
+      <c r="F70" t="n">
         <v>0</v>
       </c>
-      <c r="F70" t="inlineStr"/>
-      <c r="G70" t="inlineStr">
+      <c r="G70" t="inlineStr"/>
+      <c r="H70" t="inlineStr">
         <is>
           <t>NOT FOUND</t>
         </is>
@@ -16959,26 +17309,31 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
+          <t>156359-01</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
           <t>LANDING GEAR, ASSY, WHEEL, SECONDARY</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
+      <c r="D71" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
       </c>
-      <c r="D71" t="n">
+      <c r="E71" t="n">
         <v>2</v>
       </c>
-      <c r="E71" t="n">
+      <c r="F71" t="n">
         <v>1</v>
       </c>
-      <c r="F71" t="inlineStr">
+      <c r="G71" t="inlineStr">
         <is>
           <t>BL01000002X7 (x1)</t>
         </is>
       </c>
-      <c r="G71" t="inlineStr">
+      <c r="H71" t="inlineStr">
         <is>
           <t>NOT SATISFIED</t>
         </is>
@@ -16992,26 +17347,31 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
+          <t>156219-01</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
           <t>FAIRING, MOTOR MOUNT, LWR, OUTBD, LH</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr">
+      <c r="D72" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D72" t="n">
-        <v>1</v>
       </c>
       <c r="E72" t="n">
         <v>1</v>
       </c>
-      <c r="F72" t="inlineStr">
+      <c r="F72" t="n">
+        <v>1</v>
+      </c>
+      <c r="G72" t="inlineStr">
         <is>
           <t>BLXWFA000V4X (x1)</t>
         </is>
       </c>
-      <c r="G72" t="inlineStr">
+      <c r="H72" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -17025,194 +17385,239 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
+          <t>156220-01</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
           <t>FAIRING ASSY, MOTOR MOUNT, LWR, INBD, LH</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
+      <c r="D73" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D73" t="n">
-        <v>1</v>
       </c>
       <c r="E73" t="n">
         <v>1</v>
       </c>
-      <c r="F73" t="inlineStr">
+      <c r="F73" t="n">
+        <v>1</v>
+      </c>
+      <c r="G73" t="inlineStr">
         <is>
           <t>BLXWFA000W2U (x1)</t>
         </is>
       </c>
-      <c r="G73" t="inlineStr">
+      <c r="H73" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr"/>
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>156238-01</t>
+        </is>
+      </c>
       <c r="B74" t="inlineStr"/>
-      <c r="C74" t="inlineStr">
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
       </c>
-      <c r="D74" t="n">
+      <c r="E74" t="n">
         <v>1</v>
       </c>
-      <c r="E74" t="n">
+      <c r="F74" t="n">
         <v>0</v>
       </c>
-      <c r="F74" t="inlineStr"/>
-      <c r="G74" t="inlineStr">
+      <c r="G74" t="inlineStr"/>
+      <c r="H74" t="inlineStr">
         <is>
           <t>NOT FOUND</t>
         </is>
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr"/>
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>156217-01</t>
+        </is>
+      </c>
       <c r="B75" t="inlineStr"/>
-      <c r="C75" t="inlineStr">
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
       </c>
-      <c r="D75" t="n">
+      <c r="E75" t="n">
         <v>1</v>
       </c>
-      <c r="E75" t="n">
+      <c r="F75" t="n">
         <v>0</v>
       </c>
-      <c r="F75" t="inlineStr"/>
-      <c r="G75" t="inlineStr">
+      <c r="G75" t="inlineStr"/>
+      <c r="H75" t="inlineStr">
         <is>
           <t>NOT FOUND</t>
         </is>
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr"/>
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>150364-02</t>
+        </is>
+      </c>
       <c r="B76" t="inlineStr"/>
-      <c r="C76" t="inlineStr">
+      <c r="C76" t="inlineStr"/>
+      <c r="D76" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
       </c>
-      <c r="D76" t="n">
+      <c r="E76" t="n">
         <v>1</v>
       </c>
-      <c r="E76" t="n">
+      <c r="F76" t="n">
         <v>0</v>
       </c>
-      <c r="F76" t="inlineStr"/>
-      <c r="G76" t="inlineStr">
+      <c r="G76" t="inlineStr"/>
+      <c r="H76" t="inlineStr">
         <is>
           <t>NOT FOUND</t>
         </is>
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="inlineStr"/>
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>150352-01</t>
+        </is>
+      </c>
       <c r="B77" t="inlineStr"/>
-      <c r="C77" t="inlineStr">
+      <c r="C77" t="inlineStr"/>
+      <c r="D77" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
       </c>
-      <c r="D77" t="n">
+      <c r="E77" t="n">
         <v>1</v>
       </c>
-      <c r="E77" t="n">
+      <c r="F77" t="n">
         <v>0</v>
       </c>
-      <c r="F77" t="inlineStr"/>
-      <c r="G77" t="inlineStr">
+      <c r="G77" t="inlineStr"/>
+      <c r="H77" t="inlineStr">
         <is>
           <t>NOT FOUND</t>
         </is>
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr"/>
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>150351-01</t>
+        </is>
+      </c>
       <c r="B78" t="inlineStr"/>
-      <c r="C78" t="inlineStr">
+      <c r="C78" t="inlineStr"/>
+      <c r="D78" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
       </c>
-      <c r="D78" t="n">
+      <c r="E78" t="n">
         <v>1</v>
       </c>
-      <c r="E78" t="n">
+      <c r="F78" t="n">
         <v>0</v>
       </c>
-      <c r="F78" t="inlineStr"/>
-      <c r="G78" t="inlineStr">
+      <c r="G78" t="inlineStr"/>
+      <c r="H78" t="inlineStr">
         <is>
           <t>NOT FOUND</t>
         </is>
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="inlineStr"/>
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>150350-01</t>
+        </is>
+      </c>
       <c r="B79" t="inlineStr"/>
-      <c r="C79" t="inlineStr">
+      <c r="C79" t="inlineStr"/>
+      <c r="D79" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
       </c>
-      <c r="D79" t="n">
+      <c r="E79" t="n">
         <v>1</v>
       </c>
-      <c r="E79" t="n">
+      <c r="F79" t="n">
         <v>0</v>
       </c>
-      <c r="F79" t="inlineStr"/>
-      <c r="G79" t="inlineStr">
+      <c r="G79" t="inlineStr"/>
+      <c r="H79" t="inlineStr">
         <is>
           <t>NOT FOUND</t>
         </is>
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr"/>
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>150393-01</t>
+        </is>
+      </c>
       <c r="B80" t="inlineStr"/>
-      <c r="C80" t="inlineStr">
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
       </c>
-      <c r="D80" t="n">
+      <c r="E80" t="n">
         <v>2</v>
       </c>
-      <c r="E80" t="n">
+      <c r="F80" t="n">
         <v>0</v>
       </c>
-      <c r="F80" t="inlineStr"/>
-      <c r="G80" t="inlineStr">
+      <c r="G80" t="inlineStr"/>
+      <c r="H80" t="inlineStr">
         <is>
           <t>NOT FOUND</t>
         </is>
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr"/>
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>153336-01</t>
+        </is>
+      </c>
       <c r="B81" t="inlineStr"/>
-      <c r="C81" t="inlineStr">
+      <c r="C81" t="inlineStr"/>
+      <c r="D81" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
       </c>
-      <c r="D81" t="n">
+      <c r="E81" t="n">
         <v>1</v>
       </c>
-      <c r="E81" t="n">
+      <c r="F81" t="n">
         <v>0</v>
       </c>
-      <c r="F81" t="inlineStr"/>
-      <c r="G81" t="inlineStr">
+      <c r="G81" t="inlineStr"/>
+      <c r="H81" t="inlineStr">
         <is>
           <t>NOT FOUND</t>
         </is>
@@ -17226,26 +17631,31 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
+          <t>160138-01</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
           <t>DPC CONNECTOR BRACE</t>
         </is>
       </c>
-      <c r="C82" t="inlineStr">
+      <c r="D82" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D82" t="n">
-        <v>1</v>
       </c>
       <c r="E82" t="n">
         <v>1</v>
       </c>
-      <c r="F82" t="inlineStr">
+      <c r="F82" t="n">
+        <v>1</v>
+      </c>
+      <c r="G82" t="inlineStr">
         <is>
           <t>BL01000002LM (x1)</t>
         </is>
       </c>
-      <c r="G82" t="inlineStr">
+      <c r="H82" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>
@@ -17259,26 +17669,31 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
+          <t>159978-02</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
           <t>CABLE HOLDER, ANTENNA, SOB</t>
         </is>
       </c>
-      <c r="C83" t="inlineStr">
+      <c r="D83" t="inlineStr">
         <is>
           <t>LOT</t>
         </is>
-      </c>
-      <c r="D83" t="n">
-        <v>1</v>
       </c>
       <c r="E83" t="n">
         <v>1</v>
       </c>
-      <c r="F83" t="inlineStr">
+      <c r="F83" t="n">
+        <v>1</v>
+      </c>
+      <c r="G83" t="inlineStr">
         <is>
           <t>BL01000002HF (x1)</t>
         </is>
       </c>
-      <c r="G83" t="inlineStr">
+      <c r="H83" t="inlineStr">
         <is>
           <t>SATISFIED</t>
         </is>

</xml_diff>